<commit_message>
Add pivot table slicer refresh tests and fix related bugs.
</commit_message>
<xml_diff>
--- a/EPPlusTest/Workbooks/PivotTables/Slicers.xlsx
+++ b/EPPlusTest/Workbooks/PivotTables/Slicers.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ems\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\EPPlus\EPPlusTest\Workbooks\PivotTables\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
@@ -628,8 +628,8 @@
       <xdr:row>14</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="2" name="Posting Date 1"/>
@@ -646,7 +646,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -700,8 +700,8 @@
       <xdr:row>28</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="3" name="Amount 1"/>
@@ -718,7 +718,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -1253,7 +1253,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="C3:J39" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField showAll="0"/>
@@ -1532,7 +1532,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="B3:I39" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField showAll="0"/>
@@ -3825,7 +3825,7 @@
   <dimension ref="B3:I39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add additional slicer refresh test.
</commit_message>
<xml_diff>
--- a/EPPlusTest/Workbooks/PivotTables/Slicers.xlsx
+++ b/EPPlusTest/Workbooks/PivotTables/Slicers.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\EPPlus\EPPlusTest\Workbooks\PivotTables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ems\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="Slicer_Amount">#N/A</definedName>
@@ -23,20 +24,24 @@
     <definedName name="Slicer_Posting_Date">#N/A</definedName>
     <definedName name="Slicer_Posting_Date1">#N/A</definedName>
     <definedName name="Slicer_Source_Code">#N/A</definedName>
+    <definedName name="Slicer_Source_Code1">#N/A</definedName>
+    <definedName name="Slicer_Source_Code2">#N/A</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId4"/>
+    <pivotCache cacheId="1" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
       <x14:slicerCaches>
-        <x14:slicerCache r:id="rId5"/>
         <x14:slicerCache r:id="rId6"/>
         <x14:slicerCache r:id="rId7"/>
         <x14:slicerCache r:id="rId8"/>
         <x14:slicerCache r:id="rId9"/>
         <x14:slicerCache r:id="rId10"/>
+        <x14:slicerCache r:id="rId11"/>
+        <x14:slicerCache r:id="rId12"/>
+        <x14:slicerCache r:id="rId13"/>
       </x14:slicerCaches>
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -50,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="47">
   <si>
     <t>Entry No.</t>
   </si>
@@ -188,6 +193,9 @@
   </si>
   <si>
     <t>Column Labels</t>
+  </si>
+  <si>
+    <t>Sum of Entry No.</t>
   </si>
 </sst>
 </file>
@@ -762,6 +770,155 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="2" name="Source Code 1"/>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Source Code 1"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="4419600" y="209550"/>
+              <a:ext cx="1828800" cy="2524125"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This shape represents a slicer. Slicers are supported in Excel 2010 or later.
+If the shape was modified in an earlier version of Excel, or if the workbook was saved in Excel 2003 or earlier, the slicer cannot be used.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="3" name="Source Code 2"/>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Source Code 2"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="4410075" y="2762250"/>
+              <a:ext cx="1828800" cy="2524125"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This shape represents a slicer. Slicers are supported in Excel 2010 or later.
+If the shape was modified in an earlier version of Excel, or if the workbook was saved in Excel 2003 or earlier, the slicer cannot be used.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Evan M. Schallerer" refreshedDate="43584.391472685187" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="37">
   <cacheSource type="worksheet">
@@ -1253,7 +1410,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="C3:J39" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField showAll="0"/>
@@ -1532,7 +1689,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="B3:I39" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField showAll="0"/>
@@ -1799,6 +1956,258 @@
     </i>
   </colItems>
   <dataFields count="1">
+    <dataField name="Sum of Amount" fld="4" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="B2:D12" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
+  <pivotFields count="9">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="25">
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="8"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="4"/>
+        <item x="13"/>
+        <item x="2"/>
+        <item x="15"/>
+        <item x="3"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="14"/>
+        <item x="23"/>
+        <item x="12"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="19"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="14" showAll="0">
+      <items count="15">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="5">
+        <item x="3"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="6">
+        <item h="1" x="4"/>
+        <item h="1" x="1"/>
+        <item h="1" x="2"/>
+        <item x="3"/>
+        <item h="1" x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0" defaultSubtotal="0">
+      <items count="6">
+        <item sd="0" x="0"/>
+        <item sd="0" x="1"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="4"/>
+        <item sd="0" x="5"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0" defaultSubtotal="0">
+      <items count="4">
+        <item sd="0" x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item sd="0" x="3"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="3"/>
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="8">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="17"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="10"/>
+    </i>
+    <i r="1">
+      <x v="14"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="2">
+    <field x="8"/>
+    <field x="5"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x v="2"/>
+      <x v="3"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Amount" fld="4" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="B14:D19" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="9">
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0">
+      <items count="25">
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="8"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="4"/>
+        <item x="13"/>
+        <item x="2"/>
+        <item x="15"/>
+        <item x="3"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="14"/>
+        <item x="23"/>
+        <item x="12"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="19"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="14" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="5">
+        <item x="3"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="6">
+        <item h="1" x="4"/>
+        <item h="1" x="1"/>
+        <item x="2"/>
+        <item h="1" x="3"/>
+        <item h="1" x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="3"/>
+    <field x="5"/>
+  </rowFields>
+  <rowItems count="5">
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Entry No." fld="0" baseField="0" baseItem="0"/>
     <dataField name="Sum of Amount" fld="4" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
@@ -1997,6 +2406,44 @@
 </slicerCacheDefinition>
 </file>
 
+<file path=xl/slicerCaches/slicerCache7.xml><?xml version="1.0" encoding="utf-8"?>
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x" name="Slicer_Source_Code1" sourceName="Source Code">
+  <pivotTables>
+    <pivotTable tabId="4" name="PivotTable1"/>
+  </pivotTables>
+  <data>
+    <tabular pivotCacheId="1">
+      <items count="5">
+        <i x="4"/>
+        <i x="1"/>
+        <i x="2"/>
+        <i x="3" s="1"/>
+        <i x="0"/>
+      </items>
+    </tabular>
+  </data>
+</slicerCacheDefinition>
+</file>
+
+<file path=xl/slicerCaches/slicerCache8.xml><?xml version="1.0" encoding="utf-8"?>
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x" name="Slicer_Source_Code2" sourceName="Source Code">
+  <pivotTables>
+    <pivotTable tabId="4" name="PivotTable2"/>
+  </pivotTables>
+  <data>
+    <tabular pivotCacheId="1">
+      <items count="5">
+        <i x="4"/>
+        <i x="1"/>
+        <i x="2" s="1"/>
+        <i x="3"/>
+        <i x="0"/>
+      </items>
+    </tabular>
+  </data>
+</slicerCacheDefinition>
+</file>
+
 <file path=xl/slicers/slicer1.xml><?xml version="1.0" encoding="utf-8"?>
 <slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
   <slicer name="Posting Date" cache="Slicer_Posting_Date" caption="Posting Date" rowHeight="241300"/>
@@ -2010,6 +2457,13 @@
 <slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
   <slicer name="Posting Date 1" cache="Slicer_Posting_Date1" caption="Posting Date" rowHeight="241300"/>
   <slicer name="Amount 1" cache="Slicer_Amount1" caption="Amount" rowHeight="241300"/>
+</slicers>
+</file>
+
+<file path=xl/slicers/slicer3.xml><?xml version="1.0" encoding="utf-8"?>
+<slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <slicer name="Source Code 1" cache="Slicer_Source_Code1" caption="Source Code" rowHeight="241300"/>
+  <slicer name="Source Code 2" cache="Slicer_Source_Code2" caption="Source Code" rowHeight="241300"/>
 </slicers>
 </file>
 
@@ -2278,7 +2732,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:H40"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
@@ -3824,8 +4278,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:I39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4471,4 +4925,231 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:D19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="7" max="8" width="9" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" customWidth="1"/>
+    <col min="10" max="10" width="7" customWidth="1"/>
+    <col min="11" max="11" width="9" customWidth="1"/>
+    <col min="12" max="12" width="7" customWidth="1"/>
+    <col min="13" max="13" width="9" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="7" customWidth="1"/>
+    <col min="17" max="17" width="9" customWidth="1"/>
+    <col min="18" max="18" width="6" customWidth="1"/>
+    <col min="19" max="19" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8" customWidth="1"/>
+    <col min="21" max="21" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8" customWidth="1"/>
+    <col min="23" max="23" width="9" customWidth="1"/>
+    <col min="24" max="24" width="7" customWidth="1"/>
+    <col min="25" max="25" width="8" customWidth="1"/>
+    <col min="26" max="26" width="7" customWidth="1"/>
+    <col min="27" max="27" width="11.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="17">
+        <v>8277.85</v>
+      </c>
+      <c r="D5" s="17">
+        <v>8277.85</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="17">
+        <v>8277.85</v>
+      </c>
+      <c r="D6" s="17">
+        <v>8277.85</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="17">
+        <v>53800.14</v>
+      </c>
+      <c r="D7" s="17">
+        <v>53800.14</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="17">
+        <v>53800.14</v>
+      </c>
+      <c r="D8" s="17">
+        <v>53800.14</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="17">
+        <v>23672.06</v>
+      </c>
+      <c r="D9" s="17">
+        <v>23672.06</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="17">
+        <v>11836.03</v>
+      </c>
+      <c r="D10" s="17">
+        <v>11836.03</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="17">
+        <v>11836.03</v>
+      </c>
+      <c r="D11" s="17">
+        <v>11836.03</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="17">
+        <v>85750.05</v>
+      </c>
+      <c r="D12" s="17">
+        <v>85750.05</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="17">
+        <v>105</v>
+      </c>
+      <c r="D15" s="17">
+        <v>-53800.14</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B16" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="17">
+        <v>105</v>
+      </c>
+      <c r="D16" s="17">
+        <v>-53800.14</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="17">
+        <v>81</v>
+      </c>
+      <c r="D17" s="17">
+        <v>23672.06</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="17">
+        <v>81</v>
+      </c>
+      <c r="D18" s="17">
+        <v>23672.06</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="17">
+        <v>186</v>
+      </c>
+      <c r="D19" s="17">
+        <v>-30128.079999999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{A8765BA9-456A-4dab-B4F3-ACF838C121DE}">
+      <x14:slicerList>
+        <x14:slicer r:id="rId4"/>
+      </x14:slicerList>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>